<commit_message>
Added script for Cost Center Quota assignment.
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Vary.xlsx
+++ b/TestData/Custom_Quota_Vary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20E222B-F67F-4C6C-98CD-356B9B20D5F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B16A15-C3A2-45A9-A721-D76624EBE9A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="37">
   <si>
     <t>${quota_name}</t>
   </si>
@@ -91,36 +91,9 @@
     <t>definitionLimitsSelectControl-listbox-item-2</t>
   </si>
   <si>
-    <t>individualQuotaValuesId-row-checkbox-0</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-checkbox-1</t>
-  </si>
-  <si>
     <t>individualQuotaValuesId-row-checkbox-2</t>
   </si>
   <si>
-    <t>individualQuotaValuesId-row-checkbox-3</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-checkbox-4</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-checkbox-5</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-checkbox-6</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-checkbox-7</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-checkbox-8</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-checkbox-9</t>
-  </si>
-  <si>
     <t>Vary_Unlimited_NoColor</t>
   </si>
   <si>
@@ -151,12 +124,6 @@
     <t>Vary_Total1_Color1</t>
   </si>
   <si>
-    <t>individualQuotaValuesId-row-0-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-0-colorQuota</t>
-  </si>
-  <si>
     <t>${monthly_total_value}</t>
   </si>
   <si>
@@ -169,58 +136,10 @@
     <t>${monthly_color_id}</t>
   </si>
   <si>
-    <t>individualQuotaValuesId-row-1-totalQuota</t>
-  </si>
-  <si>
     <t>individualQuotaValuesId-row-2-totalQuota</t>
   </si>
   <si>
-    <t>individualQuotaValuesId-row-3-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-4-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-5-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-6-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-7-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-8-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-9-totalQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-1-colorQuota</t>
-  </si>
-  <si>
     <t>individualQuotaValuesId-row-2-colorQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-3-colorQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-4-colorQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-5-colorQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-6-colorQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-7-colorQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-8-colorQuota</t>
-  </si>
-  <si>
-    <t>individualQuotaValuesId-row-9-colorQuota</t>
   </si>
   <si>
     <t>Vary_Total99999_Color99999</t>
@@ -609,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,11 +539,11 @@
     <col min="1" max="1" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" customWidth="1"/>
     <col min="3" max="3" width="45.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="48" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="42.140625" style="1" bestFit="1" customWidth="1"/>
@@ -658,27 +577,27 @@
         <v>12</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -696,13 +615,13 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -710,7 +629,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>18</v>
@@ -718,29 +637,26 @@
       <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
+      <c r="G3" s="1">
+        <v>0</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="L3" s="1">
         <v>0</v>
@@ -748,19 +664,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>9</v>
@@ -769,30 +685,30 @@
         <v>11</v>
       </c>
       <c r="H4" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="L4" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="16.5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -806,66 +722,69 @@
       <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4">
-        <v>99999</v>
+      <c r="H5" s="1">
+        <v>50</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" s="4">
-        <v>99999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>35</v>
+      </c>
+      <c r="L5" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="16.5">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4">
+        <v>99999</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="L6" s="4">
+        <v>99999</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -883,13 +802,13 @@
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="J7" s="1">
         <v>50</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
@@ -897,13 +816,13 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
@@ -921,13 +840,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="L8" s="1">
         <v>0</v>
@@ -935,13 +854,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>15</v>
@@ -959,13 +878,13 @@
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="J9" s="1">
         <v>99999</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
@@ -973,13 +892,13 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>15</v>
@@ -997,13 +916,13 @@
         <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="J10" s="1">
         <v>99999</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="L10" s="1">
         <v>50</v>
@@ -1011,13 +930,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>15</v>
@@ -1035,13 +954,13 @@
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J11" s="1">
         <v>1</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="L11" s="1">
         <v>1</v>
@@ -1049,13 +968,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>15</v>
@@ -1073,41 +992,17 @@
         <v>99999</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J12" s="1">
         <v>99999</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="L12" s="1">
         <v>99999</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2"/>
@@ -1144,6 +1039,30 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1153,15 +1072,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L10"/>
+      <selection activeCell="A2" sqref="A2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -1196,10 +1120,12 @@
     <row r="8" spans="1:7" s="1" customFormat="1"/>
     <row r="9" spans="1:7" s="1" customFormat="1"/>
     <row r="10" spans="1:7" s="1" customFormat="1"/>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+    <row r="11" spans="1:7" s="1" customFormat="1"/>
+    <row r="12" spans="1:7" s="1" customFormat="1"/>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added script for Cost Center Quota assignment, Personal and Department Quota Assignment.
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Vary.xlsx
+++ b/TestData/Custom_Quota_Vary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B16A15-C3A2-45A9-A721-D76624EBE9A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E747DB4-93D0-47B8-8D37-ED7A5AD33FBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
   <si>
     <t>${quota_name}</t>
   </si>
@@ -531,7 +531,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -700,310 +700,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1">
-        <v>50</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.5">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4">
-        <v>99999</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="4">
-        <v>99999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="1">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="1">
-        <v>50</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="1">
-        <v>99999</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="1">
-        <v>99999</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="1">
-        <v>99999</v>
-      </c>
-      <c r="H10" s="1">
-        <v>50</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="1">
-        <v>99999</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1">
-        <v>99999</v>
-      </c>
-      <c r="H12" s="1">
-        <v>99999</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="1">
-        <v>99999</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" s="1">
-        <v>99999</v>
-      </c>
-    </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
@@ -1072,10 +768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,7 +784,7 @@
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1111,17 +807,384 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1"/>
-    <row r="3" spans="1:7" s="1" customFormat="1"/>
-    <row r="4" spans="1:7" s="1" customFormat="1"/>
-    <row r="5" spans="1:7" s="1" customFormat="1"/>
-    <row r="6" spans="1:7" s="1" customFormat="1"/>
-    <row r="7" spans="1:7" s="1" customFormat="1"/>
-    <row r="8" spans="1:7" s="1" customFormat="1"/>
-    <row r="9" spans="1:7" s="1" customFormat="1"/>
-    <row r="10" spans="1:7" s="1" customFormat="1"/>
-    <row r="11" spans="1:7" s="1" customFormat="1"/>
-    <row r="12" spans="1:7" s="1" customFormat="1"/>
+    <row r="2" spans="1:12" s="1" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1">
+        <v>50</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="16.5">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4">
+        <v>99999</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="4">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="1">
+        <v>50</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>99999</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="1">
+        <v>99999</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1">
+        <v>99999</v>
+      </c>
+      <c r="H9" s="1">
+        <v>50</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="1">
+        <v>99999</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1">
+        <v>99999</v>
+      </c>
+      <c r="H11" s="1">
+        <v>99999</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="1">
+        <v>99999</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="1">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1"/>
     <row r="35" spans="1:3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>

</xml_diff>

<commit_message>
Added scripts for error validations for quota
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Vary.xlsx
+++ b/TestData/Custom_Quota_Vary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E747DB4-93D0-47B8-8D37-ED7A5AD33FBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6727D90C-3CCB-4B64-9242-10D1251E983D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1192,5 +1192,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added check for presence of delete quota checkbox.
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Vary.xlsx
+++ b/TestData/Custom_Quota_Vary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93119CC-9147-442D-9BC5-9FA8CB6D360D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2219D5-E784-4BB5-9582-0832E946E38A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11505" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -697,7 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Quota related scripts
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Vary.xlsx
+++ b/TestData/Custom_Quota_Vary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FCB46B-116B-4ED5-B70C-CDBD1044A0B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA062484-4E29-4CA2-9E07-D5758D7AE693}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -519,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,17 +618,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1">
+        <v>50</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2"/>
@@ -677,6 +738,18 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -689,7 +762,7 @@
   <dimension ref="A4:L50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD18"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -892,41 +965,6 @@
         <v>99999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="15" spans="1:12" s="1" customFormat="1">
       <c r="A15" s="2" t="s">
         <v>24</v>
@@ -963,44 +1001,6 @@
       </c>
       <c r="L15" s="1">
         <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="1" customFormat="1">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="1">
-        <v>50</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="1">
-        <v>50</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1">

</xml_diff>

<commit_message>
Added quota status scripts for Python.
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Vary.xlsx
+++ b/TestData/Custom_Quota_Vary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA062484-4E29-4CA2-9E07-D5758D7AE693}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7999039D-0496-41AE-91FD-5DEAC5F0CFC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,79 +618,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="1">
-        <v>50</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="1">
-        <v>50</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
@@ -759,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
-  <dimension ref="A4:L50"/>
+  <dimension ref="A4:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="A20" sqref="A20:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1079,10 +1006,83 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+    <row r="20" spans="1:12" s="1" customFormat="1">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="1" customFormat="1">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1">
+        <v>50</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="1">
+        <v>50</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added quota status scripts for Robot framework
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Vary.xlsx
+++ b/TestData/Custom_Quota_Vary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7999039D-0496-41AE-91FD-5DEAC5F0CFC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA2F190-72D8-4281-B190-EEF3026FC171}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>${monthly_color_id}</t>
   </si>
   <si>
-    <t>Vary_Total99999_Color99999</t>
-  </si>
-  <si>
     <t>individualQuotaValuesId-row-checkbox-3</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>individualQuotaValuesId-row-3-colorQuota</t>
+  </si>
+  <si>
+    <t>Vary_Total4000_Color4000</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,16 +582,16 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
@@ -599,23 +599,23 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
+      <c r="G2" s="1">
+        <v>4000</v>
       </c>
       <c r="H2" s="1">
-        <v>1</v>
+        <v>4000</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -686,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03B8D5-BAB8-450E-A664-CABADEFF022A}">
-  <dimension ref="A4:L52"/>
+  <dimension ref="A4:L53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD21"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -710,7 +710,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
@@ -728,13 +728,13 @@
         <v>50</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" s="1">
         <v>50</v>
@@ -748,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
@@ -766,13 +766,13 @@
         <v>99999</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5" s="4">
         <v>99999</v>
@@ -786,7 +786,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -804,13 +804,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" s="1">
         <v>99999</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L8" s="1">
         <v>0</v>
@@ -824,7 +824,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>12</v>
@@ -842,144 +842,106 @@
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L10" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:12" s="1" customFormat="1">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1">
+        <v>99999</v>
+      </c>
+      <c r="H16" s="1">
+        <v>50</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="J16" s="1">
         <v>99999</v>
       </c>
-      <c r="H11" s="1">
-        <v>99999</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="K16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="1">
-        <v>99999</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="1">
-        <v>99999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1">
-      <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="1">
-        <v>99999</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="L16" s="1">
         <v>50</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="1">
-        <v>99999</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="1" customFormat="1">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>10</v>
@@ -987,102 +949,140 @@
       <c r="F18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="1" customFormat="1">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1">
         <v>1</v>
       </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="1" customFormat="1">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20" s="1">
+      <c r="L19" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="1" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="1" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1">
         <v>50</v>
       </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="1">
+        <v>50</v>
+      </c>
+      <c r="K22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J21" s="1">
-        <v>50</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>